<commit_message>
Change the numbat output files
Replace the numbat output files with the most current ones
</commit_message>
<xml_diff>
--- a/9_Miscellaneous/t1.xlsx
+++ b/9_Miscellaneous/t1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dz855/Partners HealthCare Dropbox/Nurefsan Sariipek/ImmuneEscapeTP53/TP53_ImmuneEscape/9_Miscellaneous/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFCB5F8-04A2-FB48-B9DD-2CF05255D4C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C3D664E-BB71-0848-B0C7-4FA0DFF8C48E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" xr2:uid="{A6366E64-3C3B-2243-AB5A-1CC8410567B2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="130">
   <si>
     <t>Patient_id</t>
   </si>
@@ -350,9 +350,6 @@
     <t>P28_tx</t>
   </si>
   <si>
-    <t>P28_rem</t>
-  </si>
-  <si>
     <t>P29_tx</t>
   </si>
   <si>
@@ -419,9 +416,6 @@
     <t>P25_rel</t>
   </si>
   <si>
-    <t>P26_rel</t>
-  </si>
-  <si>
     <t>P27_rel</t>
   </si>
   <si>
@@ -429,6 +423,9 @@
   </si>
   <si>
     <t>P32_rel</t>
+  </si>
+  <si>
+    <t>P28_rel</t>
   </si>
 </sst>
 </file>
@@ -814,10 +811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11086070-A44B-7A4A-BB47-98F55A4430A5}">
-  <dimension ref="A1:E89"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="165" zoomScaleNormal="165" workbookViewId="0">
-      <selection activeCell="E89" sqref="E89"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="165" zoomScaleNormal="165" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1834,7 +1831,7 @@
         <v>89</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C60">
         <v>168</v>
@@ -1885,7 +1882,7 @@
         <v>90</v>
       </c>
       <c r="B63" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C63">
         <v>522</v>
@@ -1922,7 +1919,7 @@
         <v>100</v>
       </c>
       <c r="C65">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="D65" t="s">
         <v>46</v>
@@ -1933,13 +1930,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B66" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="C66">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D66" t="s">
         <v>46</v>
@@ -1953,10 +1950,10 @@
         <v>92</v>
       </c>
       <c r="B67" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="D67" t="s">
         <v>46</v>
@@ -1970,10 +1967,10 @@
         <v>92</v>
       </c>
       <c r="B68" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
       <c r="C68">
-        <v>83</v>
+        <v>146</v>
       </c>
       <c r="D68" t="s">
         <v>46</v>
@@ -1984,13 +1981,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B69" t="s">
-        <v>128</v>
+        <v>103</v>
       </c>
       <c r="C69">
-        <v>146</v>
+        <v>0</v>
       </c>
       <c r="D69" t="s">
         <v>46</v>
@@ -2004,10 +2001,10 @@
         <v>93</v>
       </c>
       <c r="B70" t="s">
-        <v>103</v>
+        <v>129</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="D70" t="s">
         <v>46</v>
@@ -2018,13 +2015,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B71" t="s">
         <v>104</v>
       </c>
       <c r="C71">
-        <v>104</v>
+        <v>0</v>
       </c>
       <c r="D71" t="s">
         <v>46</v>
@@ -2041,7 +2038,7 @@
         <v>105</v>
       </c>
       <c r="C72">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="D72" t="s">
         <v>46</v>
@@ -2052,30 +2049,30 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>96</v>
-      </c>
-      <c r="B73" t="s">
         <v>106</v>
       </c>
+      <c r="B73" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="C73">
-        <v>90</v>
+        <v>-25</v>
       </c>
       <c r="D73" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E73" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>123</v>
       </c>
       <c r="C74">
-        <v>-25</v>
+        <v>0</v>
       </c>
       <c r="D74" t="s">
         <v>44</v>
@@ -2086,13 +2083,13 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C75">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="D75" t="s">
         <v>44</v>
@@ -2103,13 +2100,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C76">
-        <v>34</v>
+        <v>104</v>
       </c>
       <c r="D76" t="s">
         <v>44</v>
@@ -2123,10 +2120,10 @@
         <v>107</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C77">
-        <v>104</v>
+        <v>-25</v>
       </c>
       <c r="D77" t="s">
         <v>44</v>
@@ -2137,13 +2134,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>108</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>120</v>
+        <v>107</v>
+      </c>
+      <c r="B78" t="s">
+        <v>118</v>
       </c>
       <c r="C78">
-        <v>-25</v>
+        <v>0</v>
       </c>
       <c r="D78" t="s">
         <v>44</v>
@@ -2154,13 +2151,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B79" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="D79" t="s">
         <v>44</v>
@@ -2171,13 +2168,13 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B80" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C80">
-        <v>47</v>
+        <v>93</v>
       </c>
       <c r="D80" t="s">
         <v>44</v>
@@ -2191,10 +2188,10 @@
         <v>108</v>
       </c>
       <c r="B81" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C81">
-        <v>93</v>
+        <v>-25</v>
       </c>
       <c r="D81" t="s">
         <v>44</v>
@@ -2205,13 +2202,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B82" t="s">
         <v>115</v>
       </c>
       <c r="C82">
-        <v>-25</v>
+        <v>0</v>
       </c>
       <c r="D82" t="s">
         <v>44</v>
@@ -2222,13 +2219,13 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>109</v>
-      </c>
-      <c r="B83" t="s">
-        <v>116</v>
+        <v>108</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="D83" t="s">
         <v>44</v>
@@ -2239,13 +2236,13 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>109</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
+      </c>
+      <c r="B84" t="s">
+        <v>128</v>
       </c>
       <c r="C84">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="D84" t="s">
         <v>44</v>
@@ -2258,11 +2255,11 @@
       <c r="A85" t="s">
         <v>109</v>
       </c>
-      <c r="B85" t="s">
-        <v>130</v>
+      <c r="B85" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="C85">
-        <v>70</v>
+        <v>-25</v>
       </c>
       <c r="D85" t="s">
         <v>44</v>
@@ -2273,13 +2270,13 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C86">
-        <v>-25</v>
+        <v>0</v>
       </c>
       <c r="D86" t="s">
         <v>44</v>
@@ -2290,13 +2287,13 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
+        <v>109</v>
+      </c>
+      <c r="B87" t="s">
         <v>110</v>
       </c>
-      <c r="B87" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="C87">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="D87" t="s">
         <v>44</v>
@@ -2307,35 +2304,18 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>110</v>
-      </c>
-      <c r="B88" t="s">
-        <v>111</v>
+        <v>109</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="C88">
-        <v>33</v>
+        <v>258</v>
       </c>
       <c r="D88" t="s">
         <v>44</v>
       </c>
       <c r="E88" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>110</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C89">
-        <v>258</v>
-      </c>
-      <c r="D89" t="s">
-        <v>44</v>
-      </c>
-      <c r="E89" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>